<commit_message>
remove duplicate codes in MA qre when run tables
</commit_message>
<xml_diff>
--- a/tests/VN8413_ProjectName_preview.xlsx
+++ b/tests/VN8413_ProjectName_preview.xlsx
@@ -835,8 +835,12 @@
       <c r="K2" t="n">
         <v>4</v>
       </c>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
+      <c r="L2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" t="n">
+        <v>2</v>
+      </c>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="n">
         <v>4</v>

</xml_diff>

<commit_message>
merge data to ma question
</commit_message>
<xml_diff>
--- a/tests/VN8413_ProjectName_preview.xlsx
+++ b/tests/VN8413_ProjectName_preview.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BV151"/>
+  <dimension ref="A1:CH151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -800,6 +800,66 @@
           <t>Weight_Var</t>
         </is>
       </c>
+      <c r="BW1" s="1" t="inlineStr">
+        <is>
+          <t>S6a_1</t>
+        </is>
+      </c>
+      <c r="BX1" s="1" t="inlineStr">
+        <is>
+          <t>S6a_2</t>
+        </is>
+      </c>
+      <c r="BY1" s="1" t="inlineStr">
+        <is>
+          <t>S6a_3</t>
+        </is>
+      </c>
+      <c r="BZ1" s="1" t="inlineStr">
+        <is>
+          <t>S6_Merge_1</t>
+        </is>
+      </c>
+      <c r="CA1" s="1" t="inlineStr">
+        <is>
+          <t>S6_Merge_2</t>
+        </is>
+      </c>
+      <c r="CB1" s="1" t="inlineStr">
+        <is>
+          <t>S6_Merge_3</t>
+        </is>
+      </c>
+      <c r="CC1" s="1" t="inlineStr">
+        <is>
+          <t>S6_Merge_4</t>
+        </is>
+      </c>
+      <c r="CD1" s="1" t="inlineStr">
+        <is>
+          <t>S6_Merge_5</t>
+        </is>
+      </c>
+      <c r="CE1" s="1" t="inlineStr">
+        <is>
+          <t>S6_Merge_6</t>
+        </is>
+      </c>
+      <c r="CF1" s="1" t="inlineStr">
+        <is>
+          <t>S6_Merge_7</t>
+        </is>
+      </c>
+      <c r="CG1" s="1" t="inlineStr">
+        <is>
+          <t>S6_Merge_8</t>
+        </is>
+      </c>
+      <c r="CH1" s="1" t="inlineStr">
+        <is>
+          <t>S6_Merge_9</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -1010,6 +1070,28 @@
       <c r="BV2" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW2" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX2" t="inlineStr"/>
+      <c r="BY2" t="inlineStr"/>
+      <c r="BZ2" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA2" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB2" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC2" t="n">
+        <v>5</v>
+      </c>
+      <c r="CD2" t="inlineStr"/>
+      <c r="CE2" t="inlineStr"/>
+      <c r="CF2" t="inlineStr"/>
+      <c r="CG2" t="inlineStr"/>
+      <c r="CH2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -1220,6 +1302,28 @@
       <c r="BV3" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW3" t="inlineStr"/>
+      <c r="BX3" t="inlineStr"/>
+      <c r="BY3" t="inlineStr"/>
+      <c r="BZ3" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA3" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB3" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC3" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD3" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE3" t="inlineStr"/>
+      <c r="CF3" t="inlineStr"/>
+      <c r="CG3" t="inlineStr"/>
+      <c r="CH3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -1430,6 +1534,30 @@
       <c r="BV4" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW4" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX4" t="inlineStr"/>
+      <c r="BY4" t="inlineStr"/>
+      <c r="BZ4" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA4" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB4" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC4" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD4" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE4" t="inlineStr"/>
+      <c r="CF4" t="inlineStr"/>
+      <c r="CG4" t="inlineStr"/>
+      <c r="CH4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -1638,6 +1766,24 @@
       <c r="BV5" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW5" t="inlineStr"/>
+      <c r="BX5" t="inlineStr"/>
+      <c r="BY5" t="inlineStr"/>
+      <c r="BZ5" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA5" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB5" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC5" t="inlineStr"/>
+      <c r="CD5" t="inlineStr"/>
+      <c r="CE5" t="inlineStr"/>
+      <c r="CF5" t="inlineStr"/>
+      <c r="CG5" t="inlineStr"/>
+      <c r="CH5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -1848,6 +1994,28 @@
       <c r="BV6" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW6" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX6" t="inlineStr"/>
+      <c r="BY6" t="inlineStr"/>
+      <c r="BZ6" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA6" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB6" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC6" t="n">
+        <v>5</v>
+      </c>
+      <c r="CD6" t="inlineStr"/>
+      <c r="CE6" t="inlineStr"/>
+      <c r="CF6" t="inlineStr"/>
+      <c r="CG6" t="inlineStr"/>
+      <c r="CH6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -2050,6 +2218,20 @@
       <c r="BV7" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW7" t="inlineStr"/>
+      <c r="BX7" t="inlineStr"/>
+      <c r="BY7" t="inlineStr"/>
+      <c r="BZ7" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA7" t="inlineStr"/>
+      <c r="CB7" t="inlineStr"/>
+      <c r="CC7" t="inlineStr"/>
+      <c r="CD7" t="inlineStr"/>
+      <c r="CE7" t="inlineStr"/>
+      <c r="CF7" t="inlineStr"/>
+      <c r="CG7" t="inlineStr"/>
+      <c r="CH7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -2258,6 +2440,26 @@
       <c r="BV8" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW8" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX8" t="inlineStr"/>
+      <c r="BY8" t="inlineStr"/>
+      <c r="BZ8" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA8" t="n">
+        <v>4</v>
+      </c>
+      <c r="CB8" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC8" t="inlineStr"/>
+      <c r="CD8" t="inlineStr"/>
+      <c r="CE8" t="inlineStr"/>
+      <c r="CF8" t="inlineStr"/>
+      <c r="CG8" t="inlineStr"/>
+      <c r="CH8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -2466,6 +2668,26 @@
       <c r="BV9" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW9" t="inlineStr"/>
+      <c r="BX9" t="inlineStr"/>
+      <c r="BY9" t="inlineStr"/>
+      <c r="BZ9" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA9" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB9" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC9" t="n">
+        <v>5</v>
+      </c>
+      <c r="CD9" t="inlineStr"/>
+      <c r="CE9" t="inlineStr"/>
+      <c r="CF9" t="inlineStr"/>
+      <c r="CG9" t="inlineStr"/>
+      <c r="CH9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -2676,6 +2898,30 @@
       <c r="BV10" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW10" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX10" t="inlineStr"/>
+      <c r="BY10" t="inlineStr"/>
+      <c r="BZ10" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA10" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB10" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC10" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD10" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE10" t="inlineStr"/>
+      <c r="CF10" t="inlineStr"/>
+      <c r="CG10" t="inlineStr"/>
+      <c r="CH10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -2880,6 +3126,22 @@
       <c r="BV11" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW11" t="inlineStr"/>
+      <c r="BX11" t="inlineStr"/>
+      <c r="BY11" t="inlineStr"/>
+      <c r="BZ11" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA11" t="n">
+        <v>5</v>
+      </c>
+      <c r="CB11" t="inlineStr"/>
+      <c r="CC11" t="inlineStr"/>
+      <c r="CD11" t="inlineStr"/>
+      <c r="CE11" t="inlineStr"/>
+      <c r="CF11" t="inlineStr"/>
+      <c r="CG11" t="inlineStr"/>
+      <c r="CH11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -3082,6 +3344,24 @@
       <c r="BV12" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW12" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX12" t="inlineStr"/>
+      <c r="BY12" t="inlineStr"/>
+      <c r="BZ12" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA12" t="n">
+        <v>5</v>
+      </c>
+      <c r="CB12" t="inlineStr"/>
+      <c r="CC12" t="inlineStr"/>
+      <c r="CD12" t="inlineStr"/>
+      <c r="CE12" t="inlineStr"/>
+      <c r="CF12" t="inlineStr"/>
+      <c r="CG12" t="inlineStr"/>
+      <c r="CH12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -3290,6 +3570,26 @@
       <c r="BV13" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW13" t="inlineStr"/>
+      <c r="BX13" t="inlineStr"/>
+      <c r="BY13" t="inlineStr"/>
+      <c r="BZ13" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA13" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB13" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC13" t="n">
+        <v>5</v>
+      </c>
+      <c r="CD13" t="inlineStr"/>
+      <c r="CE13" t="inlineStr"/>
+      <c r="CF13" t="inlineStr"/>
+      <c r="CG13" t="inlineStr"/>
+      <c r="CH13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -3492,6 +3792,24 @@
       <c r="BV14" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW14" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX14" t="inlineStr"/>
+      <c r="BY14" t="inlineStr"/>
+      <c r="BZ14" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA14" t="n">
+        <v>5</v>
+      </c>
+      <c r="CB14" t="inlineStr"/>
+      <c r="CC14" t="inlineStr"/>
+      <c r="CD14" t="inlineStr"/>
+      <c r="CE14" t="inlineStr"/>
+      <c r="CF14" t="inlineStr"/>
+      <c r="CG14" t="inlineStr"/>
+      <c r="CH14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -3700,6 +4018,26 @@
       <c r="BV15" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW15" t="inlineStr"/>
+      <c r="BX15" t="inlineStr"/>
+      <c r="BY15" t="inlineStr"/>
+      <c r="BZ15" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA15" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB15" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC15" t="n">
+        <v>5</v>
+      </c>
+      <c r="CD15" t="inlineStr"/>
+      <c r="CE15" t="inlineStr"/>
+      <c r="CF15" t="inlineStr"/>
+      <c r="CG15" t="inlineStr"/>
+      <c r="CH15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -3910,6 +4248,30 @@
       <c r="BV16" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW16" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX16" t="inlineStr"/>
+      <c r="BY16" t="inlineStr"/>
+      <c r="BZ16" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA16" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB16" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC16" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD16" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE16" t="inlineStr"/>
+      <c r="CF16" t="inlineStr"/>
+      <c r="CG16" t="inlineStr"/>
+      <c r="CH16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -4120,6 +4482,28 @@
       <c r="BV17" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW17" t="inlineStr"/>
+      <c r="BX17" t="inlineStr"/>
+      <c r="BY17" t="inlineStr"/>
+      <c r="BZ17" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA17" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB17" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC17" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD17" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE17" t="inlineStr"/>
+      <c r="CF17" t="inlineStr"/>
+      <c r="CG17" t="inlineStr"/>
+      <c r="CH17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -4324,6 +4708,26 @@
       <c r="BV18" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW18" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX18" t="inlineStr"/>
+      <c r="BY18" t="inlineStr"/>
+      <c r="BZ18" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA18" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB18" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC18" t="inlineStr"/>
+      <c r="CD18" t="inlineStr"/>
+      <c r="CE18" t="inlineStr"/>
+      <c r="CF18" t="inlineStr"/>
+      <c r="CG18" t="inlineStr"/>
+      <c r="CH18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -4530,6 +4934,24 @@
       <c r="BV19" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW19" t="inlineStr"/>
+      <c r="BX19" t="inlineStr"/>
+      <c r="BY19" t="inlineStr"/>
+      <c r="BZ19" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA19" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB19" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC19" t="inlineStr"/>
+      <c r="CD19" t="inlineStr"/>
+      <c r="CE19" t="inlineStr"/>
+      <c r="CF19" t="inlineStr"/>
+      <c r="CG19" t="inlineStr"/>
+      <c r="CH19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -4734,6 +5156,24 @@
       <c r="BV20" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW20" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX20" t="inlineStr"/>
+      <c r="BY20" t="inlineStr"/>
+      <c r="BZ20" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA20" t="n">
+        <v>5</v>
+      </c>
+      <c r="CB20" t="inlineStr"/>
+      <c r="CC20" t="inlineStr"/>
+      <c r="CD20" t="inlineStr"/>
+      <c r="CE20" t="inlineStr"/>
+      <c r="CF20" t="inlineStr"/>
+      <c r="CG20" t="inlineStr"/>
+      <c r="CH20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -4944,6 +5384,28 @@
       <c r="BV21" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW21" t="inlineStr"/>
+      <c r="BX21" t="inlineStr"/>
+      <c r="BY21" t="inlineStr"/>
+      <c r="BZ21" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA21" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB21" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC21" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD21" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE21" t="inlineStr"/>
+      <c r="CF21" t="inlineStr"/>
+      <c r="CG21" t="inlineStr"/>
+      <c r="CH21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -5156,6 +5618,30 @@
       <c r="BV22" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW22" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX22" t="inlineStr"/>
+      <c r="BY22" t="inlineStr"/>
+      <c r="BZ22" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA22" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB22" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC22" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD22" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE22" t="inlineStr"/>
+      <c r="CF22" t="inlineStr"/>
+      <c r="CG22" t="inlineStr"/>
+      <c r="CH22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -5364,6 +5850,26 @@
       <c r="BV23" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW23" t="inlineStr"/>
+      <c r="BX23" t="inlineStr"/>
+      <c r="BY23" t="inlineStr"/>
+      <c r="BZ23" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA23" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB23" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC23" t="n">
+        <v>5</v>
+      </c>
+      <c r="CD23" t="inlineStr"/>
+      <c r="CE23" t="inlineStr"/>
+      <c r="CF23" t="inlineStr"/>
+      <c r="CG23" t="inlineStr"/>
+      <c r="CH23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -5570,6 +6076,28 @@
       <c r="BV24" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW24" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX24" t="inlineStr"/>
+      <c r="BY24" t="inlineStr"/>
+      <c r="BZ24" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA24" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB24" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC24" t="n">
+        <v>5</v>
+      </c>
+      <c r="CD24" t="inlineStr"/>
+      <c r="CE24" t="inlineStr"/>
+      <c r="CF24" t="inlineStr"/>
+      <c r="CG24" t="inlineStr"/>
+      <c r="CH24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -5780,6 +6308,28 @@
       <c r="BV25" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW25" t="inlineStr"/>
+      <c r="BX25" t="inlineStr"/>
+      <c r="BY25" t="inlineStr"/>
+      <c r="BZ25" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA25" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB25" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC25" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD25" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE25" t="inlineStr"/>
+      <c r="CF25" t="inlineStr"/>
+      <c r="CG25" t="inlineStr"/>
+      <c r="CH25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -5986,6 +6536,26 @@
       <c r="BV26" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW26" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX26" t="inlineStr"/>
+      <c r="BY26" t="inlineStr"/>
+      <c r="BZ26" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA26" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB26" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC26" t="inlineStr"/>
+      <c r="CD26" t="inlineStr"/>
+      <c r="CE26" t="inlineStr"/>
+      <c r="CF26" t="inlineStr"/>
+      <c r="CG26" t="inlineStr"/>
+      <c r="CH26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -6194,6 +6764,24 @@
       <c r="BV27" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW27" t="inlineStr"/>
+      <c r="BX27" t="inlineStr"/>
+      <c r="BY27" t="inlineStr"/>
+      <c r="BZ27" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA27" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB27" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC27" t="inlineStr"/>
+      <c r="CD27" t="inlineStr"/>
+      <c r="CE27" t="inlineStr"/>
+      <c r="CF27" t="inlineStr"/>
+      <c r="CG27" t="inlineStr"/>
+      <c r="CH27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -6406,6 +6994,30 @@
       <c r="BV28" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW28" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX28" t="inlineStr"/>
+      <c r="BY28" t="inlineStr"/>
+      <c r="BZ28" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA28" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB28" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC28" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD28" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE28" t="inlineStr"/>
+      <c r="CF28" t="inlineStr"/>
+      <c r="CG28" t="inlineStr"/>
+      <c r="CH28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -6616,6 +7228,28 @@
       <c r="BV29" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW29" t="inlineStr"/>
+      <c r="BX29" t="inlineStr"/>
+      <c r="BY29" t="inlineStr"/>
+      <c r="BZ29" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA29" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB29" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC29" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD29" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE29" t="inlineStr"/>
+      <c r="CF29" t="inlineStr"/>
+      <c r="CG29" t="inlineStr"/>
+      <c r="CH29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -6826,6 +7460,30 @@
       <c r="BV30" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW30" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX30" t="inlineStr"/>
+      <c r="BY30" t="inlineStr"/>
+      <c r="BZ30" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA30" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB30" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC30" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD30" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE30" t="inlineStr"/>
+      <c r="CF30" t="inlineStr"/>
+      <c r="CG30" t="inlineStr"/>
+      <c r="CH30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -7036,6 +7694,28 @@
       <c r="BV31" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW31" t="inlineStr"/>
+      <c r="BX31" t="inlineStr"/>
+      <c r="BY31" t="inlineStr"/>
+      <c r="BZ31" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA31" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB31" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC31" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD31" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE31" t="inlineStr"/>
+      <c r="CF31" t="inlineStr"/>
+      <c r="CG31" t="inlineStr"/>
+      <c r="CH31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -7242,6 +7922,26 @@
       <c r="BV32" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW32" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX32" t="inlineStr"/>
+      <c r="BY32" t="inlineStr"/>
+      <c r="BZ32" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA32" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB32" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC32" t="inlineStr"/>
+      <c r="CD32" t="inlineStr"/>
+      <c r="CE32" t="inlineStr"/>
+      <c r="CF32" t="inlineStr"/>
+      <c r="CG32" t="inlineStr"/>
+      <c r="CH32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -7452,6 +8152,28 @@
       <c r="BV33" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW33" t="inlineStr"/>
+      <c r="BX33" t="inlineStr"/>
+      <c r="BY33" t="inlineStr"/>
+      <c r="BZ33" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA33" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB33" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC33" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD33" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE33" t="inlineStr"/>
+      <c r="CF33" t="inlineStr"/>
+      <c r="CG33" t="inlineStr"/>
+      <c r="CH33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -7660,6 +8382,28 @@
       <c r="BV34" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW34" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX34" t="inlineStr"/>
+      <c r="BY34" t="inlineStr"/>
+      <c r="BZ34" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA34" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB34" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC34" t="n">
+        <v>5</v>
+      </c>
+      <c r="CD34" t="inlineStr"/>
+      <c r="CE34" t="inlineStr"/>
+      <c r="CF34" t="inlineStr"/>
+      <c r="CG34" t="inlineStr"/>
+      <c r="CH34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -7870,6 +8614,28 @@
       <c r="BV35" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW35" t="inlineStr"/>
+      <c r="BX35" t="inlineStr"/>
+      <c r="BY35" t="inlineStr"/>
+      <c r="BZ35" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA35" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB35" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC35" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD35" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE35" t="inlineStr"/>
+      <c r="CF35" t="inlineStr"/>
+      <c r="CG35" t="inlineStr"/>
+      <c r="CH35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -8080,6 +8846,30 @@
       <c r="BV36" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW36" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX36" t="inlineStr"/>
+      <c r="BY36" t="inlineStr"/>
+      <c r="BZ36" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA36" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB36" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC36" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD36" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE36" t="inlineStr"/>
+      <c r="CF36" t="inlineStr"/>
+      <c r="CG36" t="inlineStr"/>
+      <c r="CH36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -8286,6 +9076,24 @@
       <c r="BV37" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW37" t="inlineStr"/>
+      <c r="BX37" t="inlineStr"/>
+      <c r="BY37" t="inlineStr"/>
+      <c r="BZ37" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA37" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB37" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC37" t="inlineStr"/>
+      <c r="CD37" t="inlineStr"/>
+      <c r="CE37" t="inlineStr"/>
+      <c r="CF37" t="inlineStr"/>
+      <c r="CG37" t="inlineStr"/>
+      <c r="CH37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -8496,6 +9304,30 @@
       <c r="BV38" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW38" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX38" t="inlineStr"/>
+      <c r="BY38" t="inlineStr"/>
+      <c r="BZ38" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA38" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB38" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC38" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD38" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE38" t="inlineStr"/>
+      <c r="CF38" t="inlineStr"/>
+      <c r="CG38" t="inlineStr"/>
+      <c r="CH38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -8704,6 +9536,26 @@
       <c r="BV39" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW39" t="inlineStr"/>
+      <c r="BX39" t="inlineStr"/>
+      <c r="BY39" t="inlineStr"/>
+      <c r="BZ39" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA39" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB39" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC39" t="n">
+        <v>5</v>
+      </c>
+      <c r="CD39" t="inlineStr"/>
+      <c r="CE39" t="inlineStr"/>
+      <c r="CF39" t="inlineStr"/>
+      <c r="CG39" t="inlineStr"/>
+      <c r="CH39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -8908,6 +9760,26 @@
       <c r="BV40" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW40" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX40" t="inlineStr"/>
+      <c r="BY40" t="inlineStr"/>
+      <c r="BZ40" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA40" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB40" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC40" t="inlineStr"/>
+      <c r="CD40" t="inlineStr"/>
+      <c r="CE40" t="inlineStr"/>
+      <c r="CF40" t="inlineStr"/>
+      <c r="CG40" t="inlineStr"/>
+      <c r="CH40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -9114,6 +9986,24 @@
       <c r="BV41" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW41" t="inlineStr"/>
+      <c r="BX41" t="inlineStr"/>
+      <c r="BY41" t="inlineStr"/>
+      <c r="BZ41" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA41" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB41" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC41" t="inlineStr"/>
+      <c r="CD41" t="inlineStr"/>
+      <c r="CE41" t="inlineStr"/>
+      <c r="CF41" t="inlineStr"/>
+      <c r="CG41" t="inlineStr"/>
+      <c r="CH41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -9322,6 +10212,28 @@
       <c r="BV42" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW42" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX42" t="inlineStr"/>
+      <c r="BY42" t="inlineStr"/>
+      <c r="BZ42" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA42" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB42" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC42" t="n">
+        <v>5</v>
+      </c>
+      <c r="CD42" t="inlineStr"/>
+      <c r="CE42" t="inlineStr"/>
+      <c r="CF42" t="inlineStr"/>
+      <c r="CG42" t="inlineStr"/>
+      <c r="CH42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -9528,6 +10440,24 @@
       <c r="BV43" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW43" t="inlineStr"/>
+      <c r="BX43" t="inlineStr"/>
+      <c r="BY43" t="inlineStr"/>
+      <c r="BZ43" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA43" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB43" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC43" t="inlineStr"/>
+      <c r="CD43" t="inlineStr"/>
+      <c r="CE43" t="inlineStr"/>
+      <c r="CF43" t="inlineStr"/>
+      <c r="CG43" t="inlineStr"/>
+      <c r="CH43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -9738,6 +10668,30 @@
       <c r="BV44" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW44" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX44" t="inlineStr"/>
+      <c r="BY44" t="inlineStr"/>
+      <c r="BZ44" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA44" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB44" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC44" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD44" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE44" t="inlineStr"/>
+      <c r="CF44" t="inlineStr"/>
+      <c r="CG44" t="inlineStr"/>
+      <c r="CH44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -9944,6 +10898,24 @@
       <c r="BV45" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW45" t="inlineStr"/>
+      <c r="BX45" t="inlineStr"/>
+      <c r="BY45" t="inlineStr"/>
+      <c r="BZ45" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA45" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB45" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC45" t="inlineStr"/>
+      <c r="CD45" t="inlineStr"/>
+      <c r="CE45" t="inlineStr"/>
+      <c r="CF45" t="inlineStr"/>
+      <c r="CG45" t="inlineStr"/>
+      <c r="CH45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -10154,6 +11126,30 @@
       <c r="BV46" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW46" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX46" t="inlineStr"/>
+      <c r="BY46" t="inlineStr"/>
+      <c r="BZ46" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA46" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB46" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC46" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD46" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE46" t="inlineStr"/>
+      <c r="CF46" t="inlineStr"/>
+      <c r="CG46" t="inlineStr"/>
+      <c r="CH46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -10364,6 +11360,28 @@
       <c r="BV47" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW47" t="inlineStr"/>
+      <c r="BX47" t="inlineStr"/>
+      <c r="BY47" t="inlineStr"/>
+      <c r="BZ47" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA47" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB47" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC47" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD47" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE47" t="inlineStr"/>
+      <c r="CF47" t="inlineStr"/>
+      <c r="CG47" t="inlineStr"/>
+      <c r="CH47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -10572,6 +11590,28 @@
       <c r="BV48" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW48" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX48" t="inlineStr"/>
+      <c r="BY48" t="inlineStr"/>
+      <c r="BZ48" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA48" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB48" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC48" t="n">
+        <v>5</v>
+      </c>
+      <c r="CD48" t="inlineStr"/>
+      <c r="CE48" t="inlineStr"/>
+      <c r="CF48" t="inlineStr"/>
+      <c r="CG48" t="inlineStr"/>
+      <c r="CH48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -10782,6 +11822,28 @@
       <c r="BV49" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW49" t="inlineStr"/>
+      <c r="BX49" t="inlineStr"/>
+      <c r="BY49" t="inlineStr"/>
+      <c r="BZ49" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA49" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB49" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC49" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD49" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE49" t="inlineStr"/>
+      <c r="CF49" t="inlineStr"/>
+      <c r="CG49" t="inlineStr"/>
+      <c r="CH49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -10990,6 +12052,28 @@
       <c r="BV50" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW50" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX50" t="inlineStr"/>
+      <c r="BY50" t="inlineStr"/>
+      <c r="BZ50" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA50" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB50" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC50" t="n">
+        <v>5</v>
+      </c>
+      <c r="CD50" t="inlineStr"/>
+      <c r="CE50" t="inlineStr"/>
+      <c r="CF50" t="inlineStr"/>
+      <c r="CG50" t="inlineStr"/>
+      <c r="CH50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -11200,6 +12284,28 @@
       <c r="BV51" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW51" t="inlineStr"/>
+      <c r="BX51" t="inlineStr"/>
+      <c r="BY51" t="inlineStr"/>
+      <c r="BZ51" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA51" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB51" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC51" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD51" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE51" t="inlineStr"/>
+      <c r="CF51" t="inlineStr"/>
+      <c r="CG51" t="inlineStr"/>
+      <c r="CH51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -11410,6 +12516,30 @@
       <c r="BV52" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW52" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX52" t="inlineStr"/>
+      <c r="BY52" t="inlineStr"/>
+      <c r="BZ52" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA52" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB52" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC52" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD52" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE52" t="inlineStr"/>
+      <c r="CF52" t="inlineStr"/>
+      <c r="CG52" t="inlineStr"/>
+      <c r="CH52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -11620,6 +12750,28 @@
       <c r="BV53" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW53" t="inlineStr"/>
+      <c r="BX53" t="inlineStr"/>
+      <c r="BY53" t="inlineStr"/>
+      <c r="BZ53" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA53" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB53" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC53" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD53" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE53" t="inlineStr"/>
+      <c r="CF53" t="inlineStr"/>
+      <c r="CG53" t="inlineStr"/>
+      <c r="CH53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -11828,6 +12980,28 @@
       <c r="BV54" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW54" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX54" t="inlineStr"/>
+      <c r="BY54" t="inlineStr"/>
+      <c r="BZ54" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA54" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB54" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC54" t="n">
+        <v>5</v>
+      </c>
+      <c r="CD54" t="inlineStr"/>
+      <c r="CE54" t="inlineStr"/>
+      <c r="CF54" t="inlineStr"/>
+      <c r="CG54" t="inlineStr"/>
+      <c r="CH54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -12038,6 +13212,28 @@
       <c r="BV55" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW55" t="inlineStr"/>
+      <c r="BX55" t="inlineStr"/>
+      <c r="BY55" t="inlineStr"/>
+      <c r="BZ55" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA55" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB55" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC55" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD55" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE55" t="inlineStr"/>
+      <c r="CF55" t="inlineStr"/>
+      <c r="CG55" t="inlineStr"/>
+      <c r="CH55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -12248,6 +13444,30 @@
       <c r="BV56" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW56" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX56" t="inlineStr"/>
+      <c r="BY56" t="inlineStr"/>
+      <c r="BZ56" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA56" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB56" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC56" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD56" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE56" t="inlineStr"/>
+      <c r="CF56" t="inlineStr"/>
+      <c r="CG56" t="inlineStr"/>
+      <c r="CH56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -12456,6 +13676,26 @@
       <c r="BV57" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW57" t="inlineStr"/>
+      <c r="BX57" t="inlineStr"/>
+      <c r="BY57" t="inlineStr"/>
+      <c r="BZ57" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA57" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB57" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC57" t="n">
+        <v>5</v>
+      </c>
+      <c r="CD57" t="inlineStr"/>
+      <c r="CE57" t="inlineStr"/>
+      <c r="CF57" t="inlineStr"/>
+      <c r="CG57" t="inlineStr"/>
+      <c r="CH57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -12666,6 +13906,30 @@
       <c r="BV58" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW58" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX58" t="inlineStr"/>
+      <c r="BY58" t="inlineStr"/>
+      <c r="BZ58" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA58" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB58" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC58" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD58" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE58" t="inlineStr"/>
+      <c r="CF58" t="inlineStr"/>
+      <c r="CG58" t="inlineStr"/>
+      <c r="CH58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -12876,6 +14140,28 @@
       <c r="BV59" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW59" t="inlineStr"/>
+      <c r="BX59" t="inlineStr"/>
+      <c r="BY59" t="inlineStr"/>
+      <c r="BZ59" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA59" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB59" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC59" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD59" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE59" t="inlineStr"/>
+      <c r="CF59" t="inlineStr"/>
+      <c r="CG59" t="inlineStr"/>
+      <c r="CH59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -13086,6 +14372,30 @@
       <c r="BV60" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW60" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX60" t="inlineStr"/>
+      <c r="BY60" t="inlineStr"/>
+      <c r="BZ60" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA60" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB60" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC60" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD60" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE60" t="inlineStr"/>
+      <c r="CF60" t="inlineStr"/>
+      <c r="CG60" t="inlineStr"/>
+      <c r="CH60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -13296,6 +14606,28 @@
       <c r="BV61" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW61" t="inlineStr"/>
+      <c r="BX61" t="inlineStr"/>
+      <c r="BY61" t="inlineStr"/>
+      <c r="BZ61" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA61" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB61" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC61" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD61" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE61" t="inlineStr"/>
+      <c r="CF61" t="inlineStr"/>
+      <c r="CG61" t="inlineStr"/>
+      <c r="CH61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -13502,6 +14834,26 @@
       <c r="BV62" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW62" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX62" t="inlineStr"/>
+      <c r="BY62" t="inlineStr"/>
+      <c r="BZ62" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA62" t="n">
+        <v>4</v>
+      </c>
+      <c r="CB62" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC62" t="inlineStr"/>
+      <c r="CD62" t="inlineStr"/>
+      <c r="CE62" t="inlineStr"/>
+      <c r="CF62" t="inlineStr"/>
+      <c r="CG62" t="inlineStr"/>
+      <c r="CH62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -13706,6 +15058,22 @@
       <c r="BV63" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW63" t="inlineStr"/>
+      <c r="BX63" t="inlineStr"/>
+      <c r="BY63" t="inlineStr"/>
+      <c r="BZ63" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA63" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB63" t="inlineStr"/>
+      <c r="CC63" t="inlineStr"/>
+      <c r="CD63" t="inlineStr"/>
+      <c r="CE63" t="inlineStr"/>
+      <c r="CF63" t="inlineStr"/>
+      <c r="CG63" t="inlineStr"/>
+      <c r="CH63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -13916,6 +15284,30 @@
       <c r="BV64" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW64" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX64" t="inlineStr"/>
+      <c r="BY64" t="inlineStr"/>
+      <c r="BZ64" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA64" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB64" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC64" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD64" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE64" t="inlineStr"/>
+      <c r="CF64" t="inlineStr"/>
+      <c r="CG64" t="inlineStr"/>
+      <c r="CH64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -14122,6 +15514,22 @@
       <c r="BV65" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW65" t="inlineStr"/>
+      <c r="BX65" t="inlineStr"/>
+      <c r="BY65" t="inlineStr"/>
+      <c r="BZ65" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA65" t="n">
+        <v>5</v>
+      </c>
+      <c r="CB65" t="inlineStr"/>
+      <c r="CC65" t="inlineStr"/>
+      <c r="CD65" t="inlineStr"/>
+      <c r="CE65" t="inlineStr"/>
+      <c r="CF65" t="inlineStr"/>
+      <c r="CG65" t="inlineStr"/>
+      <c r="CH65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -14330,6 +15738,28 @@
       <c r="BV66" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW66" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX66" t="inlineStr"/>
+      <c r="BY66" t="inlineStr"/>
+      <c r="BZ66" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA66" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB66" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC66" t="n">
+        <v>5</v>
+      </c>
+      <c r="CD66" t="inlineStr"/>
+      <c r="CE66" t="inlineStr"/>
+      <c r="CF66" t="inlineStr"/>
+      <c r="CG66" t="inlineStr"/>
+      <c r="CH66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -14540,6 +15970,28 @@
       <c r="BV67" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW67" t="inlineStr"/>
+      <c r="BX67" t="inlineStr"/>
+      <c r="BY67" t="inlineStr"/>
+      <c r="BZ67" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA67" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB67" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC67" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD67" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE67" t="inlineStr"/>
+      <c r="CF67" t="inlineStr"/>
+      <c r="CG67" t="inlineStr"/>
+      <c r="CH67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -14742,6 +16194,24 @@
       <c r="BV68" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW68" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX68" t="inlineStr"/>
+      <c r="BY68" t="inlineStr"/>
+      <c r="BZ68" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA68" t="n">
+        <v>5</v>
+      </c>
+      <c r="CB68" t="inlineStr"/>
+      <c r="CC68" t="inlineStr"/>
+      <c r="CD68" t="inlineStr"/>
+      <c r="CE68" t="inlineStr"/>
+      <c r="CF68" t="inlineStr"/>
+      <c r="CG68" t="inlineStr"/>
+      <c r="CH68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -14952,6 +16422,28 @@
       <c r="BV69" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW69" t="inlineStr"/>
+      <c r="BX69" t="inlineStr"/>
+      <c r="BY69" t="inlineStr"/>
+      <c r="BZ69" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA69" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB69" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC69" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD69" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE69" t="inlineStr"/>
+      <c r="CF69" t="inlineStr"/>
+      <c r="CG69" t="inlineStr"/>
+      <c r="CH69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -15160,6 +16652,28 @@
       <c r="BV70" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW70" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX70" t="inlineStr"/>
+      <c r="BY70" t="inlineStr"/>
+      <c r="BZ70" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA70" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB70" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC70" t="n">
+        <v>5</v>
+      </c>
+      <c r="CD70" t="inlineStr"/>
+      <c r="CE70" t="inlineStr"/>
+      <c r="CF70" t="inlineStr"/>
+      <c r="CG70" t="inlineStr"/>
+      <c r="CH70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -15370,6 +16884,28 @@
       <c r="BV71" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW71" t="inlineStr"/>
+      <c r="BX71" t="inlineStr"/>
+      <c r="BY71" t="inlineStr"/>
+      <c r="BZ71" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA71" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB71" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC71" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD71" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE71" t="inlineStr"/>
+      <c r="CF71" t="inlineStr"/>
+      <c r="CG71" t="inlineStr"/>
+      <c r="CH71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -15580,6 +17116,30 @@
       <c r="BV72" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW72" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX72" t="inlineStr"/>
+      <c r="BY72" t="inlineStr"/>
+      <c r="BZ72" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA72" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB72" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC72" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD72" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE72" t="inlineStr"/>
+      <c r="CF72" t="inlineStr"/>
+      <c r="CG72" t="inlineStr"/>
+      <c r="CH72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -15790,6 +17350,28 @@
       <c r="BV73" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW73" t="inlineStr"/>
+      <c r="BX73" t="inlineStr"/>
+      <c r="BY73" t="inlineStr"/>
+      <c r="BZ73" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA73" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB73" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC73" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD73" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE73" t="inlineStr"/>
+      <c r="CF73" t="inlineStr"/>
+      <c r="CG73" t="inlineStr"/>
+      <c r="CH73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -16000,6 +17582,28 @@
       <c r="BV74" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW74" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX74" t="inlineStr"/>
+      <c r="BY74" t="inlineStr"/>
+      <c r="BZ74" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA74" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB74" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC74" t="n">
+        <v>5</v>
+      </c>
+      <c r="CD74" t="inlineStr"/>
+      <c r="CE74" t="inlineStr"/>
+      <c r="CF74" t="inlineStr"/>
+      <c r="CG74" t="inlineStr"/>
+      <c r="CH74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -16210,6 +17814,28 @@
       <c r="BV75" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW75" t="inlineStr"/>
+      <c r="BX75" t="inlineStr"/>
+      <c r="BY75" t="inlineStr"/>
+      <c r="BZ75" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA75" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB75" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC75" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD75" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE75" t="inlineStr"/>
+      <c r="CF75" t="inlineStr"/>
+      <c r="CG75" t="inlineStr"/>
+      <c r="CH75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -16420,6 +18046,28 @@
       <c r="BV76" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW76" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX76" t="inlineStr"/>
+      <c r="BY76" t="inlineStr"/>
+      <c r="BZ76" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA76" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB76" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC76" t="n">
+        <v>5</v>
+      </c>
+      <c r="CD76" t="inlineStr"/>
+      <c r="CE76" t="inlineStr"/>
+      <c r="CF76" t="inlineStr"/>
+      <c r="CG76" t="inlineStr"/>
+      <c r="CH76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -16626,6 +18274,22 @@
       <c r="BV77" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW77" t="inlineStr"/>
+      <c r="BX77" t="inlineStr"/>
+      <c r="BY77" t="inlineStr"/>
+      <c r="BZ77" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA77" t="n">
+        <v>5</v>
+      </c>
+      <c r="CB77" t="inlineStr"/>
+      <c r="CC77" t="inlineStr"/>
+      <c r="CD77" t="inlineStr"/>
+      <c r="CE77" t="inlineStr"/>
+      <c r="CF77" t="inlineStr"/>
+      <c r="CG77" t="inlineStr"/>
+      <c r="CH77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -16834,6 +18498,26 @@
       <c r="BV78" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW78" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX78" t="inlineStr"/>
+      <c r="BY78" t="inlineStr"/>
+      <c r="BZ78" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA78" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB78" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC78" t="inlineStr"/>
+      <c r="CD78" t="inlineStr"/>
+      <c r="CE78" t="inlineStr"/>
+      <c r="CF78" t="inlineStr"/>
+      <c r="CG78" t="inlineStr"/>
+      <c r="CH78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -17040,6 +18724,24 @@
       <c r="BV79" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW79" t="inlineStr"/>
+      <c r="BX79" t="inlineStr"/>
+      <c r="BY79" t="inlineStr"/>
+      <c r="BZ79" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA79" t="n">
+        <v>4</v>
+      </c>
+      <c r="CB79" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC79" t="inlineStr"/>
+      <c r="CD79" t="inlineStr"/>
+      <c r="CE79" t="inlineStr"/>
+      <c r="CF79" t="inlineStr"/>
+      <c r="CG79" t="inlineStr"/>
+      <c r="CH79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -17250,6 +18952,30 @@
       <c r="BV80" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW80" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX80" t="inlineStr"/>
+      <c r="BY80" t="inlineStr"/>
+      <c r="BZ80" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA80" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB80" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC80" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD80" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE80" t="inlineStr"/>
+      <c r="CF80" t="inlineStr"/>
+      <c r="CG80" t="inlineStr"/>
+      <c r="CH80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -17452,6 +19178,20 @@
       <c r="BV81" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW81" t="inlineStr"/>
+      <c r="BX81" t="inlineStr"/>
+      <c r="BY81" t="inlineStr"/>
+      <c r="BZ81" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA81" t="inlineStr"/>
+      <c r="CB81" t="inlineStr"/>
+      <c r="CC81" t="inlineStr"/>
+      <c r="CD81" t="inlineStr"/>
+      <c r="CE81" t="inlineStr"/>
+      <c r="CF81" t="inlineStr"/>
+      <c r="CG81" t="inlineStr"/>
+      <c r="CH81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -17660,6 +19400,28 @@
       <c r="BV82" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW82" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX82" t="inlineStr"/>
+      <c r="BY82" t="inlineStr"/>
+      <c r="BZ82" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA82" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB82" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC82" t="n">
+        <v>5</v>
+      </c>
+      <c r="CD82" t="inlineStr"/>
+      <c r="CE82" t="inlineStr"/>
+      <c r="CF82" t="inlineStr"/>
+      <c r="CG82" t="inlineStr"/>
+      <c r="CH82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -17870,6 +19632,28 @@
       <c r="BV83" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW83" t="inlineStr"/>
+      <c r="BX83" t="inlineStr"/>
+      <c r="BY83" t="inlineStr"/>
+      <c r="BZ83" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA83" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB83" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC83" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD83" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE83" t="inlineStr"/>
+      <c r="CF83" t="inlineStr"/>
+      <c r="CG83" t="inlineStr"/>
+      <c r="CH83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -18078,6 +19862,26 @@
       <c r="BV84" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW84" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX84" t="inlineStr"/>
+      <c r="BY84" t="inlineStr"/>
+      <c r="BZ84" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA84" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB84" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC84" t="inlineStr"/>
+      <c r="CD84" t="inlineStr"/>
+      <c r="CE84" t="inlineStr"/>
+      <c r="CF84" t="inlineStr"/>
+      <c r="CG84" t="inlineStr"/>
+      <c r="CH84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -18286,6 +20090,24 @@
       <c r="BV85" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW85" t="inlineStr"/>
+      <c r="BX85" t="inlineStr"/>
+      <c r="BY85" t="inlineStr"/>
+      <c r="BZ85" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA85" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB85" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC85" t="inlineStr"/>
+      <c r="CD85" t="inlineStr"/>
+      <c r="CE85" t="inlineStr"/>
+      <c r="CF85" t="inlineStr"/>
+      <c r="CG85" t="inlineStr"/>
+      <c r="CH85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -18494,6 +20316,30 @@
       <c r="BV86" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW86" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX86" t="inlineStr"/>
+      <c r="BY86" t="inlineStr"/>
+      <c r="BZ86" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA86" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB86" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC86" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD86" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE86" t="inlineStr"/>
+      <c r="CF86" t="inlineStr"/>
+      <c r="CG86" t="inlineStr"/>
+      <c r="CH86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -18702,6 +20548,24 @@
       <c r="BV87" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW87" t="inlineStr"/>
+      <c r="BX87" t="inlineStr"/>
+      <c r="BY87" t="inlineStr"/>
+      <c r="BZ87" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA87" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB87" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC87" t="inlineStr"/>
+      <c r="CD87" t="inlineStr"/>
+      <c r="CE87" t="inlineStr"/>
+      <c r="CF87" t="inlineStr"/>
+      <c r="CG87" t="inlineStr"/>
+      <c r="CH87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -18910,6 +20774,26 @@
       <c r="BV88" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW88" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX88" t="inlineStr"/>
+      <c r="BY88" t="inlineStr"/>
+      <c r="BZ88" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA88" t="n">
+        <v>4</v>
+      </c>
+      <c r="CB88" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC88" t="inlineStr"/>
+      <c r="CD88" t="inlineStr"/>
+      <c r="CE88" t="inlineStr"/>
+      <c r="CF88" t="inlineStr"/>
+      <c r="CG88" t="inlineStr"/>
+      <c r="CH88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -19116,6 +21000,24 @@
       <c r="BV89" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW89" t="inlineStr"/>
+      <c r="BX89" t="inlineStr"/>
+      <c r="BY89" t="inlineStr"/>
+      <c r="BZ89" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA89" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB89" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC89" t="inlineStr"/>
+      <c r="CD89" t="inlineStr"/>
+      <c r="CE89" t="inlineStr"/>
+      <c r="CF89" t="inlineStr"/>
+      <c r="CG89" t="inlineStr"/>
+      <c r="CH89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -19324,6 +21226,26 @@
       <c r="BV90" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW90" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX90" t="inlineStr"/>
+      <c r="BY90" t="inlineStr"/>
+      <c r="BZ90" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA90" t="n">
+        <v>4</v>
+      </c>
+      <c r="CB90" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC90" t="inlineStr"/>
+      <c r="CD90" t="inlineStr"/>
+      <c r="CE90" t="inlineStr"/>
+      <c r="CF90" t="inlineStr"/>
+      <c r="CG90" t="inlineStr"/>
+      <c r="CH90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -19532,6 +21454,26 @@
       <c r="BV91" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW91" t="inlineStr"/>
+      <c r="BX91" t="inlineStr"/>
+      <c r="BY91" t="inlineStr"/>
+      <c r="BZ91" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA91" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB91" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC91" t="n">
+        <v>5</v>
+      </c>
+      <c r="CD91" t="inlineStr"/>
+      <c r="CE91" t="inlineStr"/>
+      <c r="CF91" t="inlineStr"/>
+      <c r="CG91" t="inlineStr"/>
+      <c r="CH91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -19742,6 +21684,28 @@
       <c r="BV92" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW92" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX92" t="inlineStr"/>
+      <c r="BY92" t="inlineStr"/>
+      <c r="BZ92" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA92" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB92" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC92" t="n">
+        <v>5</v>
+      </c>
+      <c r="CD92" t="inlineStr"/>
+      <c r="CE92" t="inlineStr"/>
+      <c r="CF92" t="inlineStr"/>
+      <c r="CG92" t="inlineStr"/>
+      <c r="CH92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -19948,6 +21912,22 @@
       <c r="BV93" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW93" t="inlineStr"/>
+      <c r="BX93" t="inlineStr"/>
+      <c r="BY93" t="inlineStr"/>
+      <c r="BZ93" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA93" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB93" t="inlineStr"/>
+      <c r="CC93" t="inlineStr"/>
+      <c r="CD93" t="inlineStr"/>
+      <c r="CE93" t="inlineStr"/>
+      <c r="CF93" t="inlineStr"/>
+      <c r="CG93" t="inlineStr"/>
+      <c r="CH93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -20154,6 +22134,26 @@
       <c r="BV94" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW94" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX94" t="inlineStr"/>
+      <c r="BY94" t="inlineStr"/>
+      <c r="BZ94" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA94" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB94" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC94" t="inlineStr"/>
+      <c r="CD94" t="inlineStr"/>
+      <c r="CE94" t="inlineStr"/>
+      <c r="CF94" t="inlineStr"/>
+      <c r="CG94" t="inlineStr"/>
+      <c r="CH94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -20360,6 +22360,22 @@
       <c r="BV95" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW95" t="inlineStr"/>
+      <c r="BX95" t="inlineStr"/>
+      <c r="BY95" t="inlineStr"/>
+      <c r="BZ95" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA95" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB95" t="inlineStr"/>
+      <c r="CC95" t="inlineStr"/>
+      <c r="CD95" t="inlineStr"/>
+      <c r="CE95" t="inlineStr"/>
+      <c r="CF95" t="inlineStr"/>
+      <c r="CG95" t="inlineStr"/>
+      <c r="CH95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -20570,6 +22586,28 @@
       <c r="BV96" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW96" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX96" t="inlineStr"/>
+      <c r="BY96" t="inlineStr"/>
+      <c r="BZ96" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA96" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB96" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC96" t="n">
+        <v>5</v>
+      </c>
+      <c r="CD96" t="inlineStr"/>
+      <c r="CE96" t="inlineStr"/>
+      <c r="CF96" t="inlineStr"/>
+      <c r="CG96" t="inlineStr"/>
+      <c r="CH96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -20776,6 +22814,22 @@
       <c r="BV97" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW97" t="inlineStr"/>
+      <c r="BX97" t="inlineStr"/>
+      <c r="BY97" t="inlineStr"/>
+      <c r="BZ97" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA97" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB97" t="inlineStr"/>
+      <c r="CC97" t="inlineStr"/>
+      <c r="CD97" t="inlineStr"/>
+      <c r="CE97" t="inlineStr"/>
+      <c r="CF97" t="inlineStr"/>
+      <c r="CG97" t="inlineStr"/>
+      <c r="CH97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -20982,6 +23036,26 @@
       <c r="BV98" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW98" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX98" t="inlineStr"/>
+      <c r="BY98" t="inlineStr"/>
+      <c r="BZ98" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA98" t="n">
+        <v>4</v>
+      </c>
+      <c r="CB98" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC98" t="inlineStr"/>
+      <c r="CD98" t="inlineStr"/>
+      <c r="CE98" t="inlineStr"/>
+      <c r="CF98" t="inlineStr"/>
+      <c r="CG98" t="inlineStr"/>
+      <c r="CH98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -21188,6 +23262,22 @@
       <c r="BV99" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW99" t="inlineStr"/>
+      <c r="BX99" t="inlineStr"/>
+      <c r="BY99" t="inlineStr"/>
+      <c r="BZ99" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA99" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB99" t="inlineStr"/>
+      <c r="CC99" t="inlineStr"/>
+      <c r="CD99" t="inlineStr"/>
+      <c r="CE99" t="inlineStr"/>
+      <c r="CF99" t="inlineStr"/>
+      <c r="CG99" t="inlineStr"/>
+      <c r="CH99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -21396,6 +23486,28 @@
       <c r="BV100" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW100" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX100" t="inlineStr"/>
+      <c r="BY100" t="inlineStr"/>
+      <c r="BZ100" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA100" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB100" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC100" t="n">
+        <v>5</v>
+      </c>
+      <c r="CD100" t="inlineStr"/>
+      <c r="CE100" t="inlineStr"/>
+      <c r="CF100" t="inlineStr"/>
+      <c r="CG100" t="inlineStr"/>
+      <c r="CH100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -21604,6 +23716,24 @@
       <c r="BV101" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW101" t="inlineStr"/>
+      <c r="BX101" t="inlineStr"/>
+      <c r="BY101" t="inlineStr"/>
+      <c r="BZ101" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA101" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB101" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC101" t="inlineStr"/>
+      <c r="CD101" t="inlineStr"/>
+      <c r="CE101" t="inlineStr"/>
+      <c r="CF101" t="inlineStr"/>
+      <c r="CG101" t="inlineStr"/>
+      <c r="CH101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -21810,6 +23940,26 @@
       <c r="BV102" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW102" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX102" t="inlineStr"/>
+      <c r="BY102" t="inlineStr"/>
+      <c r="BZ102" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA102" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB102" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC102" t="inlineStr"/>
+      <c r="CD102" t="inlineStr"/>
+      <c r="CE102" t="inlineStr"/>
+      <c r="CF102" t="inlineStr"/>
+      <c r="CG102" t="inlineStr"/>
+      <c r="CH102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -22018,6 +24168,24 @@
       <c r="BV103" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW103" t="inlineStr"/>
+      <c r="BX103" t="inlineStr"/>
+      <c r="BY103" t="inlineStr"/>
+      <c r="BZ103" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA103" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB103" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC103" t="inlineStr"/>
+      <c r="CD103" t="inlineStr"/>
+      <c r="CE103" t="inlineStr"/>
+      <c r="CF103" t="inlineStr"/>
+      <c r="CG103" t="inlineStr"/>
+      <c r="CH103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -22226,6 +24394,26 @@
       <c r="BV104" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW104" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX104" t="inlineStr"/>
+      <c r="BY104" t="inlineStr"/>
+      <c r="BZ104" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA104" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB104" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC104" t="inlineStr"/>
+      <c r="CD104" t="inlineStr"/>
+      <c r="CE104" t="inlineStr"/>
+      <c r="CF104" t="inlineStr"/>
+      <c r="CG104" t="inlineStr"/>
+      <c r="CH104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -22432,6 +24620,22 @@
       <c r="BV105" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW105" t="inlineStr"/>
+      <c r="BX105" t="inlineStr"/>
+      <c r="BY105" t="inlineStr"/>
+      <c r="BZ105" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA105" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB105" t="inlineStr"/>
+      <c r="CC105" t="inlineStr"/>
+      <c r="CD105" t="inlineStr"/>
+      <c r="CE105" t="inlineStr"/>
+      <c r="CF105" t="inlineStr"/>
+      <c r="CG105" t="inlineStr"/>
+      <c r="CH105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
@@ -22636,6 +24840,24 @@
       <c r="BV106" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW106" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX106" t="inlineStr"/>
+      <c r="BY106" t="inlineStr"/>
+      <c r="BZ106" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA106" t="n">
+        <v>5</v>
+      </c>
+      <c r="CB106" t="inlineStr"/>
+      <c r="CC106" t="inlineStr"/>
+      <c r="CD106" t="inlineStr"/>
+      <c r="CE106" t="inlineStr"/>
+      <c r="CF106" t="inlineStr"/>
+      <c r="CG106" t="inlineStr"/>
+      <c r="CH106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
@@ -22844,6 +25066,24 @@
       <c r="BV107" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW107" t="inlineStr"/>
+      <c r="BX107" t="inlineStr"/>
+      <c r="BY107" t="inlineStr"/>
+      <c r="BZ107" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA107" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB107" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC107" t="inlineStr"/>
+      <c r="CD107" t="inlineStr"/>
+      <c r="CE107" t="inlineStr"/>
+      <c r="CF107" t="inlineStr"/>
+      <c r="CG107" t="inlineStr"/>
+      <c r="CH107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
@@ -23052,6 +25292,28 @@
       <c r="BV108" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW108" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX108" t="inlineStr"/>
+      <c r="BY108" t="inlineStr"/>
+      <c r="BZ108" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA108" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB108" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC108" t="n">
+        <v>5</v>
+      </c>
+      <c r="CD108" t="inlineStr"/>
+      <c r="CE108" t="inlineStr"/>
+      <c r="CF108" t="inlineStr"/>
+      <c r="CG108" t="inlineStr"/>
+      <c r="CH108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
@@ -23260,6 +25522,24 @@
       <c r="BV109" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW109" t="inlineStr"/>
+      <c r="BX109" t="inlineStr"/>
+      <c r="BY109" t="inlineStr"/>
+      <c r="BZ109" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA109" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB109" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC109" t="inlineStr"/>
+      <c r="CD109" t="inlineStr"/>
+      <c r="CE109" t="inlineStr"/>
+      <c r="CF109" t="inlineStr"/>
+      <c r="CG109" t="inlineStr"/>
+      <c r="CH109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -23468,6 +25748,28 @@
       <c r="BV110" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW110" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX110" t="inlineStr"/>
+      <c r="BY110" t="inlineStr"/>
+      <c r="BZ110" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA110" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB110" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC110" t="n">
+        <v>5</v>
+      </c>
+      <c r="CD110" t="inlineStr"/>
+      <c r="CE110" t="inlineStr"/>
+      <c r="CF110" t="inlineStr"/>
+      <c r="CG110" t="inlineStr"/>
+      <c r="CH110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -23676,6 +25978,24 @@
       <c r="BV111" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW111" t="inlineStr"/>
+      <c r="BX111" t="inlineStr"/>
+      <c r="BY111" t="inlineStr"/>
+      <c r="BZ111" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA111" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB111" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC111" t="inlineStr"/>
+      <c r="CD111" t="inlineStr"/>
+      <c r="CE111" t="inlineStr"/>
+      <c r="CF111" t="inlineStr"/>
+      <c r="CG111" t="inlineStr"/>
+      <c r="CH111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
@@ -23882,6 +26202,26 @@
       <c r="BV112" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW112" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX112" t="inlineStr"/>
+      <c r="BY112" t="inlineStr"/>
+      <c r="BZ112" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA112" t="n">
+        <v>4</v>
+      </c>
+      <c r="CB112" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC112" t="inlineStr"/>
+      <c r="CD112" t="inlineStr"/>
+      <c r="CE112" t="inlineStr"/>
+      <c r="CF112" t="inlineStr"/>
+      <c r="CG112" t="inlineStr"/>
+      <c r="CH112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
@@ -24092,6 +26432,26 @@
       <c r="BV113" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW113" t="inlineStr"/>
+      <c r="BX113" t="inlineStr"/>
+      <c r="BY113" t="inlineStr"/>
+      <c r="BZ113" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA113" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB113" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC113" t="n">
+        <v>5</v>
+      </c>
+      <c r="CD113" t="inlineStr"/>
+      <c r="CE113" t="inlineStr"/>
+      <c r="CF113" t="inlineStr"/>
+      <c r="CG113" t="inlineStr"/>
+      <c r="CH113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
@@ -24304,6 +26664,30 @@
       <c r="BV114" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW114" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX114" t="inlineStr"/>
+      <c r="BY114" t="inlineStr"/>
+      <c r="BZ114" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA114" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB114" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC114" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD114" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE114" t="inlineStr"/>
+      <c r="CF114" t="inlineStr"/>
+      <c r="CG114" t="inlineStr"/>
+      <c r="CH114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
@@ -24512,6 +26896,24 @@
       <c r="BV115" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW115" t="inlineStr"/>
+      <c r="BX115" t="inlineStr"/>
+      <c r="BY115" t="inlineStr"/>
+      <c r="BZ115" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA115" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB115" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC115" t="inlineStr"/>
+      <c r="CD115" t="inlineStr"/>
+      <c r="CE115" t="inlineStr"/>
+      <c r="CF115" t="inlineStr"/>
+      <c r="CG115" t="inlineStr"/>
+      <c r="CH115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
@@ -24718,6 +27120,28 @@
       <c r="BV116" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW116" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX116" t="inlineStr"/>
+      <c r="BY116" t="inlineStr"/>
+      <c r="BZ116" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA116" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB116" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC116" t="n">
+        <v>5</v>
+      </c>
+      <c r="CD116" t="inlineStr"/>
+      <c r="CE116" t="inlineStr"/>
+      <c r="CF116" t="inlineStr"/>
+      <c r="CG116" t="inlineStr"/>
+      <c r="CH116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
@@ -24926,6 +27350,24 @@
       <c r="BV117" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW117" t="inlineStr"/>
+      <c r="BX117" t="inlineStr"/>
+      <c r="BY117" t="inlineStr"/>
+      <c r="BZ117" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA117" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB117" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC117" t="inlineStr"/>
+      <c r="CD117" t="inlineStr"/>
+      <c r="CE117" t="inlineStr"/>
+      <c r="CF117" t="inlineStr"/>
+      <c r="CG117" t="inlineStr"/>
+      <c r="CH117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
@@ -25136,6 +27578,30 @@
       <c r="BV118" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW118" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX118" t="inlineStr"/>
+      <c r="BY118" t="inlineStr"/>
+      <c r="BZ118" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA118" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB118" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC118" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD118" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE118" t="inlineStr"/>
+      <c r="CF118" t="inlineStr"/>
+      <c r="CG118" t="inlineStr"/>
+      <c r="CH118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
@@ -25342,6 +27808,22 @@
       <c r="BV119" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW119" t="inlineStr"/>
+      <c r="BX119" t="inlineStr"/>
+      <c r="BY119" t="inlineStr"/>
+      <c r="BZ119" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA119" t="n">
+        <v>5</v>
+      </c>
+      <c r="CB119" t="inlineStr"/>
+      <c r="CC119" t="inlineStr"/>
+      <c r="CD119" t="inlineStr"/>
+      <c r="CE119" t="inlineStr"/>
+      <c r="CF119" t="inlineStr"/>
+      <c r="CG119" t="inlineStr"/>
+      <c r="CH119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
@@ -25548,6 +28030,24 @@
       <c r="BV120" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW120" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX120" t="inlineStr"/>
+      <c r="BY120" t="inlineStr"/>
+      <c r="BZ120" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA120" t="n">
+        <v>5</v>
+      </c>
+      <c r="CB120" t="inlineStr"/>
+      <c r="CC120" t="inlineStr"/>
+      <c r="CD120" t="inlineStr"/>
+      <c r="CE120" t="inlineStr"/>
+      <c r="CF120" t="inlineStr"/>
+      <c r="CG120" t="inlineStr"/>
+      <c r="CH120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
@@ -25756,6 +28256,24 @@
       <c r="BV121" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW121" t="inlineStr"/>
+      <c r="BX121" t="inlineStr"/>
+      <c r="BY121" t="inlineStr"/>
+      <c r="BZ121" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA121" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB121" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC121" t="inlineStr"/>
+      <c r="CD121" t="inlineStr"/>
+      <c r="CE121" t="inlineStr"/>
+      <c r="CF121" t="inlineStr"/>
+      <c r="CG121" t="inlineStr"/>
+      <c r="CH121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
@@ -25964,6 +28482,28 @@
       <c r="BV122" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW122" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX122" t="inlineStr"/>
+      <c r="BY122" t="inlineStr"/>
+      <c r="BZ122" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA122" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB122" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC122" t="n">
+        <v>5</v>
+      </c>
+      <c r="CD122" t="inlineStr"/>
+      <c r="CE122" t="inlineStr"/>
+      <c r="CF122" t="inlineStr"/>
+      <c r="CG122" t="inlineStr"/>
+      <c r="CH122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
@@ -26174,6 +28714,26 @@
       <c r="BV123" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW123" t="inlineStr"/>
+      <c r="BX123" t="inlineStr"/>
+      <c r="BY123" t="inlineStr"/>
+      <c r="BZ123" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA123" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB123" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC123" t="n">
+        <v>5</v>
+      </c>
+      <c r="CD123" t="inlineStr"/>
+      <c r="CE123" t="inlineStr"/>
+      <c r="CF123" t="inlineStr"/>
+      <c r="CG123" t="inlineStr"/>
+      <c r="CH123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
@@ -26380,6 +28940,26 @@
       <c r="BV124" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW124" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX124" t="inlineStr"/>
+      <c r="BY124" t="inlineStr"/>
+      <c r="BZ124" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA124" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB124" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC124" t="inlineStr"/>
+      <c r="CD124" t="inlineStr"/>
+      <c r="CE124" t="inlineStr"/>
+      <c r="CF124" t="inlineStr"/>
+      <c r="CG124" t="inlineStr"/>
+      <c r="CH124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
@@ -26588,6 +29168,24 @@
       <c r="BV125" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW125" t="inlineStr"/>
+      <c r="BX125" t="inlineStr"/>
+      <c r="BY125" t="inlineStr"/>
+      <c r="BZ125" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA125" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB125" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC125" t="inlineStr"/>
+      <c r="CD125" t="inlineStr"/>
+      <c r="CE125" t="inlineStr"/>
+      <c r="CF125" t="inlineStr"/>
+      <c r="CG125" t="inlineStr"/>
+      <c r="CH125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
@@ -26796,6 +29394,28 @@
       <c r="BV126" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW126" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX126" t="inlineStr"/>
+      <c r="BY126" t="inlineStr"/>
+      <c r="BZ126" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA126" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB126" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC126" t="n">
+        <v>5</v>
+      </c>
+      <c r="CD126" t="inlineStr"/>
+      <c r="CE126" t="inlineStr"/>
+      <c r="CF126" t="inlineStr"/>
+      <c r="CG126" t="inlineStr"/>
+      <c r="CH126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
@@ -27008,6 +29628,28 @@
       <c r="BV127" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW127" t="inlineStr"/>
+      <c r="BX127" t="inlineStr"/>
+      <c r="BY127" t="inlineStr"/>
+      <c r="BZ127" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA127" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB127" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC127" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD127" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE127" t="inlineStr"/>
+      <c r="CF127" t="inlineStr"/>
+      <c r="CG127" t="inlineStr"/>
+      <c r="CH127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
@@ -27218,6 +29860,30 @@
       <c r="BV128" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW128" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX128" t="inlineStr"/>
+      <c r="BY128" t="inlineStr"/>
+      <c r="BZ128" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA128" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB128" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC128" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD128" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE128" t="inlineStr"/>
+      <c r="CF128" t="inlineStr"/>
+      <c r="CG128" t="inlineStr"/>
+      <c r="CH128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
@@ -27426,6 +30092,24 @@
       <c r="BV129" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW129" t="inlineStr"/>
+      <c r="BX129" t="inlineStr"/>
+      <c r="BY129" t="inlineStr"/>
+      <c r="BZ129" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA129" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB129" t="n">
+        <v>4</v>
+      </c>
+      <c r="CC129" t="inlineStr"/>
+      <c r="CD129" t="inlineStr"/>
+      <c r="CE129" t="inlineStr"/>
+      <c r="CF129" t="inlineStr"/>
+      <c r="CG129" t="inlineStr"/>
+      <c r="CH129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
@@ -27636,6 +30320,30 @@
       <c r="BV130" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW130" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX130" t="inlineStr"/>
+      <c r="BY130" t="inlineStr"/>
+      <c r="BZ130" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA130" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB130" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC130" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD130" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE130" t="inlineStr"/>
+      <c r="CF130" t="inlineStr"/>
+      <c r="CG130" t="inlineStr"/>
+      <c r="CH130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
@@ -27846,6 +30554,26 @@
       <c r="BV131" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW131" t="inlineStr"/>
+      <c r="BX131" t="inlineStr"/>
+      <c r="BY131" t="inlineStr"/>
+      <c r="BZ131" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA131" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB131" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC131" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD131" t="inlineStr"/>
+      <c r="CE131" t="inlineStr"/>
+      <c r="CF131" t="inlineStr"/>
+      <c r="CG131" t="inlineStr"/>
+      <c r="CH131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
@@ -28052,6 +30780,26 @@
       <c r="BV132" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW132" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX132" t="inlineStr"/>
+      <c r="BY132" t="inlineStr"/>
+      <c r="BZ132" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA132" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB132" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC132" t="inlineStr"/>
+      <c r="CD132" t="inlineStr"/>
+      <c r="CE132" t="inlineStr"/>
+      <c r="CF132" t="inlineStr"/>
+      <c r="CG132" t="inlineStr"/>
+      <c r="CH132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
@@ -28258,6 +31006,22 @@
       <c r="BV133" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW133" t="inlineStr"/>
+      <c r="BX133" t="inlineStr"/>
+      <c r="BY133" t="inlineStr"/>
+      <c r="BZ133" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA133" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB133" t="inlineStr"/>
+      <c r="CC133" t="inlineStr"/>
+      <c r="CD133" t="inlineStr"/>
+      <c r="CE133" t="inlineStr"/>
+      <c r="CF133" t="inlineStr"/>
+      <c r="CG133" t="inlineStr"/>
+      <c r="CH133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
@@ -28464,6 +31228,26 @@
       <c r="BV134" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW134" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX134" t="inlineStr"/>
+      <c r="BY134" t="inlineStr"/>
+      <c r="BZ134" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA134" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB134" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC134" t="inlineStr"/>
+      <c r="CD134" t="inlineStr"/>
+      <c r="CE134" t="inlineStr"/>
+      <c r="CF134" t="inlineStr"/>
+      <c r="CG134" t="inlineStr"/>
+      <c r="CH134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
@@ -28670,6 +31454,22 @@
       <c r="BV135" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW135" t="inlineStr"/>
+      <c r="BX135" t="inlineStr"/>
+      <c r="BY135" t="inlineStr"/>
+      <c r="BZ135" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA135" t="n">
+        <v>5</v>
+      </c>
+      <c r="CB135" t="inlineStr"/>
+      <c r="CC135" t="inlineStr"/>
+      <c r="CD135" t="inlineStr"/>
+      <c r="CE135" t="inlineStr"/>
+      <c r="CF135" t="inlineStr"/>
+      <c r="CG135" t="inlineStr"/>
+      <c r="CH135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
@@ -28880,6 +31680,30 @@
       <c r="BV136" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW136" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX136" t="inlineStr"/>
+      <c r="BY136" t="inlineStr"/>
+      <c r="BZ136" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA136" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB136" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC136" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD136" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE136" t="inlineStr"/>
+      <c r="CF136" t="inlineStr"/>
+      <c r="CG136" t="inlineStr"/>
+      <c r="CH136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
@@ -29082,6 +31906,20 @@
       <c r="BV137" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW137" t="inlineStr"/>
+      <c r="BX137" t="inlineStr"/>
+      <c r="BY137" t="inlineStr"/>
+      <c r="BZ137" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA137" t="inlineStr"/>
+      <c r="CB137" t="inlineStr"/>
+      <c r="CC137" t="inlineStr"/>
+      <c r="CD137" t="inlineStr"/>
+      <c r="CE137" t="inlineStr"/>
+      <c r="CF137" t="inlineStr"/>
+      <c r="CG137" t="inlineStr"/>
+      <c r="CH137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
@@ -29288,6 +32126,26 @@
       <c r="BV138" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW138" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX138" t="inlineStr"/>
+      <c r="BY138" t="inlineStr"/>
+      <c r="BZ138" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA138" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB138" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC138" t="inlineStr"/>
+      <c r="CD138" t="inlineStr"/>
+      <c r="CE138" t="inlineStr"/>
+      <c r="CF138" t="inlineStr"/>
+      <c r="CG138" t="inlineStr"/>
+      <c r="CH138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
@@ -29496,6 +32354,24 @@
       <c r="BV139" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW139" t="inlineStr"/>
+      <c r="BX139" t="inlineStr"/>
+      <c r="BY139" t="inlineStr"/>
+      <c r="BZ139" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA139" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB139" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC139" t="inlineStr"/>
+      <c r="CD139" t="inlineStr"/>
+      <c r="CE139" t="inlineStr"/>
+      <c r="CF139" t="inlineStr"/>
+      <c r="CG139" t="inlineStr"/>
+      <c r="CH139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
@@ -29702,6 +32578,26 @@
       <c r="BV140" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW140" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX140" t="inlineStr"/>
+      <c r="BY140" t="inlineStr"/>
+      <c r="BZ140" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA140" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB140" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC140" t="inlineStr"/>
+      <c r="CD140" t="inlineStr"/>
+      <c r="CE140" t="inlineStr"/>
+      <c r="CF140" t="inlineStr"/>
+      <c r="CG140" t="inlineStr"/>
+      <c r="CH140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
@@ -29912,6 +32808,28 @@
       <c r="BV141" t="n">
         <v>0.9</v>
       </c>
+      <c r="BW141" t="inlineStr"/>
+      <c r="BX141" t="inlineStr"/>
+      <c r="BY141" t="inlineStr"/>
+      <c r="BZ141" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA141" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB141" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC141" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD141" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE141" t="inlineStr"/>
+      <c r="CF141" t="inlineStr"/>
+      <c r="CG141" t="inlineStr"/>
+      <c r="CH141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
@@ -30118,6 +33036,26 @@
       <c r="BV142" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW142" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX142" t="inlineStr"/>
+      <c r="BY142" t="inlineStr"/>
+      <c r="BZ142" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA142" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB142" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC142" t="inlineStr"/>
+      <c r="CD142" t="inlineStr"/>
+      <c r="CE142" t="inlineStr"/>
+      <c r="CF142" t="inlineStr"/>
+      <c r="CG142" t="inlineStr"/>
+      <c r="CH142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
@@ -30324,6 +33262,22 @@
       <c r="BV143" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW143" t="inlineStr"/>
+      <c r="BX143" t="inlineStr"/>
+      <c r="BY143" t="inlineStr"/>
+      <c r="BZ143" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA143" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB143" t="inlineStr"/>
+      <c r="CC143" t="inlineStr"/>
+      <c r="CD143" t="inlineStr"/>
+      <c r="CE143" t="inlineStr"/>
+      <c r="CF143" t="inlineStr"/>
+      <c r="CG143" t="inlineStr"/>
+      <c r="CH143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
@@ -30530,6 +33484,26 @@
       <c r="BV144" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW144" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX144" t="inlineStr"/>
+      <c r="BY144" t="inlineStr"/>
+      <c r="BZ144" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA144" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB144" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC144" t="inlineStr"/>
+      <c r="CD144" t="inlineStr"/>
+      <c r="CE144" t="inlineStr"/>
+      <c r="CF144" t="inlineStr"/>
+      <c r="CG144" t="inlineStr"/>
+      <c r="CH144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
@@ -30738,6 +33712,24 @@
       <c r="BV145" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW145" t="inlineStr"/>
+      <c r="BX145" t="inlineStr"/>
+      <c r="BY145" t="inlineStr"/>
+      <c r="BZ145" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA145" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB145" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC145" t="inlineStr"/>
+      <c r="CD145" t="inlineStr"/>
+      <c r="CE145" t="inlineStr"/>
+      <c r="CF145" t="inlineStr"/>
+      <c r="CG145" t="inlineStr"/>
+      <c r="CH145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
@@ -30948,6 +33940,30 @@
       <c r="BV146" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW146" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX146" t="inlineStr"/>
+      <c r="BY146" t="inlineStr"/>
+      <c r="BZ146" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA146" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB146" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC146" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD146" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE146" t="inlineStr"/>
+      <c r="CF146" t="inlineStr"/>
+      <c r="CG146" t="inlineStr"/>
+      <c r="CH146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
@@ -31154,6 +34170,22 @@
       <c r="BV147" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW147" t="inlineStr"/>
+      <c r="BX147" t="inlineStr"/>
+      <c r="BY147" t="inlineStr"/>
+      <c r="BZ147" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA147" t="n">
+        <v>4</v>
+      </c>
+      <c r="CB147" t="inlineStr"/>
+      <c r="CC147" t="inlineStr"/>
+      <c r="CD147" t="inlineStr"/>
+      <c r="CE147" t="inlineStr"/>
+      <c r="CF147" t="inlineStr"/>
+      <c r="CG147" t="inlineStr"/>
+      <c r="CH147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
@@ -31360,6 +34392,26 @@
       <c r="BV148" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW148" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX148" t="inlineStr"/>
+      <c r="BY148" t="inlineStr"/>
+      <c r="BZ148" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA148" t="n">
+        <v>3</v>
+      </c>
+      <c r="CB148" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC148" t="inlineStr"/>
+      <c r="CD148" t="inlineStr"/>
+      <c r="CE148" t="inlineStr"/>
+      <c r="CF148" t="inlineStr"/>
+      <c r="CG148" t="inlineStr"/>
+      <c r="CH148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
@@ -31568,6 +34620,24 @@
       <c r="BV149" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW149" t="inlineStr"/>
+      <c r="BX149" t="inlineStr"/>
+      <c r="BY149" t="inlineStr"/>
+      <c r="BZ149" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA149" t="n">
+        <v>4</v>
+      </c>
+      <c r="CB149" t="n">
+        <v>5</v>
+      </c>
+      <c r="CC149" t="inlineStr"/>
+      <c r="CD149" t="inlineStr"/>
+      <c r="CE149" t="inlineStr"/>
+      <c r="CF149" t="inlineStr"/>
+      <c r="CG149" t="inlineStr"/>
+      <c r="CH149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
@@ -31780,6 +34850,30 @@
       <c r="BV150" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW150" t="n">
+        <v>5</v>
+      </c>
+      <c r="BX150" t="inlineStr"/>
+      <c r="BY150" t="inlineStr"/>
+      <c r="BZ150" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA150" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB150" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC150" t="n">
+        <v>4</v>
+      </c>
+      <c r="CD150" t="n">
+        <v>5</v>
+      </c>
+      <c r="CE150" t="inlineStr"/>
+      <c r="CF150" t="inlineStr"/>
+      <c r="CG150" t="inlineStr"/>
+      <c r="CH150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
@@ -31990,6 +35084,26 @@
       <c r="BV151" t="n">
         <v>1.1</v>
       </c>
+      <c r="BW151" t="inlineStr"/>
+      <c r="BX151" t="inlineStr"/>
+      <c r="BY151" t="inlineStr"/>
+      <c r="BZ151" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA151" t="n">
+        <v>2</v>
+      </c>
+      <c r="CB151" t="n">
+        <v>3</v>
+      </c>
+      <c r="CC151" t="n">
+        <v>5</v>
+      </c>
+      <c r="CD151" t="inlineStr"/>
+      <c r="CE151" t="inlineStr"/>
+      <c r="CF151" t="inlineStr"/>
+      <c r="CG151" t="inlineStr"/>
+      <c r="CH151" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -32002,7 +35116,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -33857,6 +36971,306 @@
         </is>
       </c>
     </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>S6a_1</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>S6a. New</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>MA</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>{'1': 'Bia lon/chai', '2': 'Cà phê hòa tan/ uống liền', '3': 'Nước ngọt có ga', '4': 'Nước uống đóng chai', '5': 'Nước tăng lực', '6': 'Tôi không uống loại nào ở trên'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>S6a_2</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>S6a. New</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>MA</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>{'1': 'Bia lon/chai', '2': 'Cà phê hòa tan/ uống liền', '3': 'Nước ngọt có ga', '4': 'Nước uống đóng chai', '5': 'Nước tăng lực', '6': 'Tôi không uống loại nào ở trên'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>S6a_3</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>S6a. New</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>MA</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>{'1': 'Bia lon/chai', '2': 'Cà phê hòa tan/ uống liền', '3': 'Nước ngọt có ga', '4': 'Nước uống đóng chai', '5': 'Nước tăng lực', '6': 'Tôi không uống loại nào ở trên'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>S6_Merge_1</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>S6. Merge</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>MA</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>{'1': 'Bia lon/chai', '2': 'Cà phê hòa tan/ uống liền', '3': 'Nước ngọt có ga', '4': 'Nước uống đóng chai', '5': 'Nước tăng lực', '6': 'Tôi không uống loại nào ở trên'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>S6_Merge_2</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>S6. Merge</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>MA</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>{'1': 'Bia lon/chai', '2': 'Cà phê hòa tan/ uống liền', '3': 'Nước ngọt có ga', '4': 'Nước uống đóng chai', '5': 'Nước tăng lực', '6': 'Tôi không uống loại nào ở trên'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>S6_Merge_3</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>S6. Merge</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>MA</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>{'1': 'Bia lon/chai', '2': 'Cà phê hòa tan/ uống liền', '3': 'Nước ngọt có ga', '4': 'Nước uống đóng chai', '5': 'Nước tăng lực', '6': 'Tôi không uống loại nào ở trên'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>S6_Merge_4</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>S6. Merge</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>MA</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>{'1': 'Bia lon/chai', '2': 'Cà phê hòa tan/ uống liền', '3': 'Nước ngọt có ga', '4': 'Nước uống đóng chai', '5': 'Nước tăng lực', '6': 'Tôi không uống loại nào ở trên'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>S6_Merge_5</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>S6. Merge</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>MA</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>{'1': 'Bia lon/chai', '2': 'Cà phê hòa tan/ uống liền', '3': 'Nước ngọt có ga', '4': 'Nước uống đóng chai', '5': 'Nước tăng lực', '6': 'Tôi không uống loại nào ở trên'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>S6_Merge_6</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>S6. Merge</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>MA</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>{'1': 'Bia lon/chai', '2': 'Cà phê hòa tan/ uống liền', '3': 'Nước ngọt có ga', '4': 'Nước uống đóng chai', '5': 'Nước tăng lực', '6': 'Tôi không uống loại nào ở trên'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>S6_Merge_7</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>S6. Merge</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>MA</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>{'1': 'Bia lon/chai', '2': 'Cà phê hòa tan/ uống liền', '3': 'Nước ngọt có ga', '4': 'Nước uống đóng chai', '5': 'Nước tăng lực', '6': 'Tôi không uống loại nào ở trên'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>S6_Merge_8</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>S6. Merge</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>MA</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>{'1': 'Bia lon/chai', '2': 'Cà phê hòa tan/ uống liền', '3': 'Nước ngọt có ga', '4': 'Nước uống đóng chai', '5': 'Nước tăng lực', '6': 'Tôi không uống loại nào ở trên'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>S6_Merge_9</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>S6. Merge</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>MA</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>{'1': 'Bia lon/chai', '2': 'Cà phê hòa tan/ uống liền', '3': 'Nước ngọt có ga', '4': 'Nước uống đóng chai', '5': 'Nước tăng lực', '6': 'Tôi không uống loại nào ở trên'}</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>